<commit_message>
subindo atualizacao do timescore e execução de experiencia
</commit_message>
<xml_diff>
--- a/PredLig/src/Documentation/Time Score Exemple Execution.xlsx
+++ b/PredLig/src/Documentation/Time Score Exemple Execution.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TimeScore" sheetId="1" state="visible" r:id="rId2"/>
@@ -179,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:N21"/>
+  <dimension ref="B4:P21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -233,7 +233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
@@ -241,19 +241,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">2 / ((1/B5) + (1/C5))</f>
@@ -261,23 +261,45 @@
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">(H5 - F5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K5" s="0" t="n">
         <f aca="false">(1 - G5) ^ J5</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">I5*K5</f>
-        <v>0.166666666666667</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="M5" s="0" t="n">
         <f aca="false">ABS( (D5 - E5)) + 1</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N5" s="0" t="n">
         <f aca="false">L5 / M5</f>
-        <v>0.0555555555555556</v>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <f aca="false">N5+N5</f>
+        <v>1.33333333333333</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="0" t="n">
+        <f aca="false">(B5+C5)/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">I8*K5</f>
+        <v>0.75</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">L8/M8</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,7 +327,7 @@
   </sheetPr>
   <dimension ref="B4:K10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>